<commit_message>
Changes based on Phase 2 discussion on 7/16/2020
Improved documentation. Now have diagnoses and medications since -365 days, lab values since -60 days, and procedures since 0 days from admission date.
</commit_message>
<xml_diff>
--- a/4CE_Phase2.0_File_Descriptions.xlsx
+++ b/4CE_Phase2.0_File_Descriptions.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GWEBER\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GWEBER\Desktop\Covidi2b2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14805" windowHeight="12045"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26175" windowHeight="17175"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="117">
   <si>
     <t>siteid</t>
   </si>
@@ -52,12 +52,6 @@
     <t>calendar_date</t>
   </si>
   <si>
-    <t>4CE Phase 1.1</t>
-  </si>
-  <si>
-    <t>Instructions</t>
-  </si>
-  <si>
     <t>General Notes</t>
   </si>
   <si>
@@ -118,9 +112,6 @@
     <t>6) Save the four new CSV files generated by the Phase 2.0 script.</t>
   </si>
   <si>
-    <t>7) Run Phase 2.0 Phython/R analyses.</t>
-  </si>
-  <si>
     <t>4) Run the Phase 1.1 database script WITHOUT OBFUSCATION and save the six Phase 1.1 CSV files.</t>
   </si>
   <si>
@@ -130,12 +121,6 @@
     <t>We expect that at most sites, the two patient_num's will be identical, in which case this file is optional.</t>
   </si>
   <si>
-    <t>File #4: PatientMapping.csv</t>
-  </si>
-  <si>
-    <t>File #1: PatientSummary.csv</t>
-  </si>
-  <si>
     <t>This file has one row per patient.</t>
   </si>
   <si>
@@ -151,18 +136,12 @@
     <t>A "still_in_hospital" flag indicates if the patient was still in the hospital when the script was run, which means the final outcome (discharge vs death) is not yet known.</t>
   </si>
   <si>
-    <t>File #2: PatientClinicalCourse.csv</t>
-  </si>
-  <si>
     <t>This file has one row per patient and "days_since_admission".</t>
   </si>
   <si>
     <t>It indicates which days the patient was in the hospital and when the patient became severe or died.</t>
   </si>
   <si>
-    <t>File #3: PatientObservations.csv</t>
-  </si>
-  <si>
     <t>This file has one row per patient, days_since_admission, and "concept".</t>
   </si>
   <si>
@@ -172,18 +151,6 @@
     <t>If a patient has the same lab repeated in the same day, then the value in this CSV file is the mean of all the test results from that day.</t>
   </si>
   <si>
-    <t>The file contains all labs and procedures since the patients were admitted. It does not contain any prior labs or procedures.</t>
-  </si>
-  <si>
-    <t>The file contains the first instance of each diagnosis and medication code since the patient was admitted.</t>
-  </si>
-  <si>
-    <t>It also contains the first instance of each diagnosis and medication code between -365 and -15 days before admission.</t>
-  </si>
-  <si>
-    <t>Thus, each diagnosis and medication code can be listed twice in the file (once before COVID and once after COVID).</t>
-  </si>
-  <si>
     <t>This is a draft! 4CE sites are not yet expected to run the Phase 2.0 script yet.</t>
   </si>
   <si>
@@ -262,12 +229,6 @@
     <t>same as Phase 1.1: the earliest admission date between 7 days before and 14 days after the first COVID-19 positive test result</t>
   </si>
   <si>
-    <t>0 = day of admission</t>
-  </si>
-  <si>
-    <t>if the patient is still in the hospital, then "1/1/1900"</t>
-  </si>
-  <si>
     <t>1 = the patient is still in the hospital, 0 = the patient left the hospital either discharged or deceased</t>
   </si>
   <si>
@@ -316,9 +277,6 @@
     <t>0 = never dead or not yet dead, 1 = deceased</t>
   </si>
   <si>
-    <t>DIAG-ICD9, DIAG-ICD10, PROC-ICD9, PROC-ICD10, LAB-LOINC, MED-CLASS</t>
-  </si>
-  <si>
     <t>the specific code</t>
   </si>
   <si>
@@ -352,7 +310,73 @@
     <t>LAB-LOINC</t>
   </si>
   <si>
-    <t xml:space="preserve">Concepts include (1) first three character ICD9/10 diagnoses, (2) Phase 1.1 LOINC labs, (3) Phase 1.1 medication classes, and (4) ICD9/10 procedure codes used in Phase 1.1 to determine severity </t>
+    <t>4CE Phase 2</t>
+  </si>
+  <si>
+    <t>File #1: LocalPatientSummary.csv</t>
+  </si>
+  <si>
+    <t>File #2: LocalPatientClinicalCourse.csv</t>
+  </si>
+  <si>
+    <t>File #3: LocalPatientObservations.csv</t>
+  </si>
+  <si>
+    <t>File #4: LocalPatientMapping.csv</t>
+  </si>
+  <si>
+    <t>Make sure you read the 4CE Phase 1.1 documentation before reading this file.</t>
+  </si>
+  <si>
+    <t>Read 4CE Phase 1.1 Documentation First!</t>
+  </si>
+  <si>
+    <t>You will need to generate the 4CE Phase 1.1 files before running the Phase 2 scripts.</t>
+  </si>
+  <si>
+    <t>The 4CE Phase 1.1 documentation defines the COVID-19 cohort and the various codes used in Phase 2.</t>
+  </si>
+  <si>
+    <t>Instructions for 4CE Phase 2</t>
+  </si>
+  <si>
+    <t>7) Run Phase 2.0 R/Python analyses.</t>
+  </si>
+  <si>
+    <t>Column names must be lower case because R is case sensitive.</t>
+  </si>
+  <si>
+    <t>Concepts include (1) first three character ICD9/10 diagnoses, (2) Phase 1.1 medication classes, (3) Phase 1.1 LOINC labs, and (4) ICD9/10 procedure codes used in Phase 1.1 to determine severity.</t>
+  </si>
+  <si>
+    <t>Diagnoses and medications start at day -365 (one year before the patient was admitted) and go through the current date.</t>
+  </si>
+  <si>
+    <t>Lab test results start at day -60 (two months before the patient was admitted) and go through the current date.</t>
+  </si>
+  <si>
+    <t>Procedure codes start at day 0 (the day of admission) and go through the current date.</t>
+  </si>
+  <si>
+    <t>Note that this files does not contain every observation that a patient has. It only contains the rolled-up concepts that were quality checked in Phase 1.1.</t>
+  </si>
+  <si>
+    <t>The 4CE Phase 1.1 documentation is located at https://github.com/GriffinWeber/covid19i2b2</t>
+  </si>
+  <si>
+    <t>number of days between the admission date and the date when this file is generated (0 if this file is created the day the patient is admitted)</t>
+  </si>
+  <si>
+    <t>0 = day of admission; 1 = one day after admission; 2 = two days after admission; etc.</t>
+  </si>
+  <si>
+    <t>0 = day of admission (values should be &gt;= -365 for diagnoses and medications, &gt;= -60 for labs, and &gt;= 0 for procedures)</t>
+  </si>
+  <si>
+    <t>DIAG-ICD9, DIAG-ICD10, MED-CLASS, LAB-LOINC, PROC-ICD9, PROC-ICD10</t>
+  </si>
+  <si>
+    <t>use "1/1/1900" if the patient is still in the hospital when this file is generated</t>
   </si>
 </sst>
 </file>
@@ -460,7 +484,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -507,6 +531,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -788,7 +819,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L49"/>
+  <dimension ref="A1:L56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -799,12 +830,12 @@
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>8</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>44008</v>
+        <v>44037</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -812,7 +843,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -826,199 +857,298 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="25"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+    </row>
+    <row r="6" spans="1:12" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>9</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
+      <c r="A7" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>27</v>
-      </c>
+      <c r="A8" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>31</v>
-      </c>
+      <c r="A9" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>10</v>
+      <c r="A10" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>73</v>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>35</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>41</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>44</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>46</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>50</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>33</v>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1042,16 +1172,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1059,13 +1189,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -1073,35 +1203,35 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D5" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -1110,147 +1240,147 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>78</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D7" t="s">
-        <v>79</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D9" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D11" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D13" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D14" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s">
         <v>3</v>
       </c>
       <c r="C15" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" t="s">
         <v>74</v>
-      </c>
-      <c r="D15" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1258,13 +1388,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D18" t="s">
         <v>5</v>
@@ -1272,21 +1402,21 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C19" s="15" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>6</v>
@@ -1295,63 +1425,63 @@
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>78</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B22" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C22" s="15" t="s">
         <v>4</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C23" s="15" t="s">
         <v>4</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C24" s="15" t="s">
         <v>4</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1359,13 +1489,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B26" t="s">
         <v>0</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D26" t="s">
         <v>5</v>
@@ -1373,21 +1503,21 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C27" s="15" t="s">
         <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>6</v>
@@ -1396,49 +1526,49 @@
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D29" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D30" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1446,13 +1576,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B33" t="s">
         <v>0</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D33" t="s">
         <v>5</v>
@@ -1460,30 +1590,30 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C34" s="15" t="s">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B35" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C35" s="15" t="s">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1509,7 +1639,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N33"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1531,7 +1661,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -1552,31 +1682,31 @@
         <v>0</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="K2" s="10" t="s">
         <v>1</v>
@@ -1588,12 +1718,12 @@
         <v>3</v>
       </c>
       <c r="N2" s="10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="11">
         <v>1</v>
@@ -1623,13 +1753,13 @@
         <v>0</v>
       </c>
       <c r="K3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="M3" s="11" t="s">
         <v>22</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="M3" s="11" t="s">
-        <v>24</v>
       </c>
       <c r="N3" s="11">
         <v>1</v>
@@ -1637,7 +1767,7 @@
     </row>
     <row r="4" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B4" s="11">
         <v>2</v>
@@ -1667,13 +1797,13 @@
         <v>1</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="N4" s="11">
         <v>1</v>
@@ -1681,7 +1811,7 @@
     </row>
     <row r="5" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B5" s="11">
         <v>3</v>
@@ -1711,13 +1841,13 @@
         <v>0</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="N5" s="11">
         <v>1</v>
@@ -1740,7 +1870,7 @@
     </row>
     <row r="7" spans="1:14" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -1761,7 +1891,7 @@
         <v>0</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>6</v>
@@ -1770,13 +1900,13 @@
         <v>7</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
@@ -1788,7 +1918,7 @@
     </row>
     <row r="9" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B9" s="11">
         <v>1</v>
@@ -1818,7 +1948,7 @@
     </row>
     <row r="10" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B10" s="11">
         <v>1</v>
@@ -1848,7 +1978,7 @@
     </row>
     <row r="11" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" s="11">
         <v>1</v>
@@ -1860,7 +1990,7 @@
         <v>43917</v>
       </c>
       <c r="E11" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="22">
         <v>0</v>
@@ -1878,16 +2008,16 @@
     </row>
     <row r="12" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B12" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" s="22">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D12" s="12">
-        <v>43922</v>
+        <v>43918</v>
       </c>
       <c r="E12" s="22">
         <v>1</v>
@@ -1908,22 +2038,22 @@
     </row>
     <row r="13" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" s="22">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D13" s="12">
-        <v>43923</v>
+        <v>43919</v>
       </c>
       <c r="E13" s="22">
         <v>1</v>
       </c>
       <c r="F13" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" s="22">
         <v>0</v>
@@ -1938,25 +2068,25 @@
     </row>
     <row r="14" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B14" s="11">
         <v>2</v>
       </c>
       <c r="C14" s="22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D14" s="12">
-        <v>43924</v>
+        <v>43922</v>
       </c>
       <c r="E14" s="22">
         <v>1</v>
       </c>
       <c r="F14" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
@@ -1967,12 +2097,27 @@
       <c r="N14" s="9"/>
     </row>
     <row r="15" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
+      <c r="A15" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="11">
+        <v>2</v>
+      </c>
+      <c r="C15" s="22">
+        <v>1</v>
+      </c>
+      <c r="D15" s="12">
+        <v>43923</v>
+      </c>
+      <c r="E15" s="22">
+        <v>1</v>
+      </c>
+      <c r="F15" s="22">
+        <v>1</v>
+      </c>
+      <c r="G15" s="22">
+        <v>0</v>
+      </c>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
@@ -1981,182 +2126,175 @@
       <c r="M15" s="9"/>
       <c r="N15" s="9"/>
     </row>
-    <row r="16" spans="1:14" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-    </row>
-    <row r="17" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="10" t="s">
+    <row r="16" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="11">
+        <v>2</v>
+      </c>
+      <c r="C16" s="22">
+        <v>2</v>
+      </c>
+      <c r="D16" s="12">
+        <v>43924</v>
+      </c>
+      <c r="E16" s="22">
+        <v>1</v>
+      </c>
+      <c r="F16" s="22">
+        <v>1</v>
+      </c>
+      <c r="G16" s="22">
+        <v>1</v>
+      </c>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+    </row>
+    <row r="17" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="11">
+        <v>2</v>
+      </c>
+      <c r="C17" s="22">
+        <v>3</v>
+      </c>
+      <c r="D17" s="12">
+        <v>43925</v>
+      </c>
+      <c r="E17" s="22">
+        <v>0</v>
+      </c>
+      <c r="F17" s="22">
+        <v>1</v>
+      </c>
+      <c r="G17" s="22">
+        <v>1</v>
+      </c>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+    </row>
+    <row r="18" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="11">
+        <v>2</v>
+      </c>
+      <c r="C18" s="22">
+        <v>4</v>
+      </c>
+      <c r="D18" s="12">
+        <v>43926</v>
+      </c>
+      <c r="E18" s="22">
+        <v>0</v>
+      </c>
+      <c r="F18" s="22">
+        <v>1</v>
+      </c>
+      <c r="G18" s="22">
+        <v>1</v>
+      </c>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+    </row>
+    <row r="19" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+    </row>
+    <row r="20" spans="1:14" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+    </row>
+    <row r="21" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-    </row>
-    <row r="18" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="23">
-        <v>1</v>
-      </c>
-      <c r="C18" s="23">
-        <v>-134</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="F18" s="23">
-        <v>-999</v>
-      </c>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="24"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="24"/>
-      <c r="N18" s="24"/>
-    </row>
-    <row r="19" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="23">
-        <v>1</v>
-      </c>
-      <c r="C19" s="23">
-        <v>1</v>
-      </c>
-      <c r="D19" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="E19" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="F19" s="23">
-        <v>-999</v>
-      </c>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="24"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="24"/>
-      <c r="N19" s="24"/>
-    </row>
-    <row r="20" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="23">
-        <v>2</v>
-      </c>
-      <c r="C20" s="23">
-        <v>0</v>
-      </c>
-      <c r="D20" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="E20" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="F20" s="23">
-        <v>6.1</v>
-      </c>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="24"/>
-      <c r="N20" s="24"/>
-    </row>
-    <row r="21" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="23">
-        <v>2</v>
-      </c>
-      <c r="C21" s="23">
-        <v>1</v>
-      </c>
-      <c r="D21" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="E21" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="F21" s="23">
-        <v>6.4</v>
-      </c>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="24"/>
-      <c r="K21" s="24"/>
-      <c r="L21" s="24"/>
-      <c r="M21" s="24"/>
-      <c r="N21" s="24"/>
+      <c r="F21" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
     </row>
     <row r="22" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B22" s="23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C22" s="23">
-        <v>2</v>
+        <v>-134</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>21</v>
+        <v>92</v>
       </c>
       <c r="F22" s="23">
-        <v>7.2</v>
+        <v>-999</v>
       </c>
       <c r="G22" s="24"/>
       <c r="H22" s="24"/>
@@ -2168,11 +2306,24 @@
       <c r="N22" s="24"/>
     </row>
     <row r="23" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
+      <c r="A23" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="23">
+        <v>1</v>
+      </c>
+      <c r="C23" s="23">
+        <v>1</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="F23" s="23">
+        <v>-999</v>
+      </c>
       <c r="G23" s="24"/>
       <c r="H23" s="24"/>
       <c r="I23" s="24"/>
@@ -2182,130 +2333,155 @@
       <c r="M23" s="24"/>
       <c r="N23" s="24"/>
     </row>
-    <row r="24" spans="1:14" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
-    </row>
-    <row r="25" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8"/>
-    </row>
-    <row r="26" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" s="11">
+    <row r="24" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="23">
+        <v>2</v>
+      </c>
+      <c r="C24" s="23">
+        <v>0</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="23">
+        <v>6.1</v>
+      </c>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="24"/>
+      <c r="N24" s="24"/>
+    </row>
+    <row r="25" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="23">
+        <v>2</v>
+      </c>
+      <c r="C25" s="23">
+        <v>1</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="23">
+        <v>6.4</v>
+      </c>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
+      <c r="L25" s="24"/>
+      <c r="M25" s="24"/>
+      <c r="N25" s="24"/>
+    </row>
+    <row r="26" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="23">
+        <v>2</v>
+      </c>
+      <c r="C26" s="23">
+        <v>2</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="E26" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="23">
+        <v>7.2</v>
+      </c>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="24"/>
+      <c r="N26" s="24"/>
+    </row>
+    <row r="27" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
+      <c r="K27" s="24"/>
+      <c r="L27" s="24"/>
+      <c r="M27" s="24"/>
+      <c r="N27" s="24"/>
+    </row>
+    <row r="28" spans="1:14" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+    </row>
+    <row r="29" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+    </row>
+    <row r="30" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="11">
         <v>10001051</v>
       </c>
-      <c r="C26" s="11">
-        <v>1</v>
-      </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="9"/>
-    </row>
-    <row r="27" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" s="11">
-        <v>10008430</v>
-      </c>
-      <c r="C27" s="11">
-        <v>2</v>
-      </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="9"/>
-    </row>
-    <row r="28" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="11">
-        <v>10005824</v>
-      </c>
-      <c r="C28" s="11">
-        <v>3</v>
-      </c>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="9"/>
-    </row>
-    <row r="29" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-    </row>
-    <row r="30" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
+      <c r="C30" s="11">
+        <v>1</v>
+      </c>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
@@ -2319,8 +2495,15 @@
       <c r="N30" s="9"/>
     </row>
     <row r="31" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
+      <c r="A31" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="11">
+        <v>10008430</v>
+      </c>
+      <c r="C31" s="11">
+        <v>2</v>
+      </c>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
@@ -2334,8 +2517,15 @@
       <c r="N31" s="9"/>
     </row>
     <row r="32" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
+      <c r="A32" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" s="11">
+        <v>10005824</v>
+      </c>
+      <c r="C32" s="11">
+        <v>3</v>
+      </c>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
@@ -2363,6 +2553,66 @@
       <c r="M33" s="9"/>
       <c r="N33" s="9"/>
     </row>
+    <row r="34" spans="2:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="9"/>
+      <c r="M34" s="9"/>
+      <c r="N34" s="9"/>
+    </row>
+    <row r="35" spans="2:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="9"/>
+      <c r="M35" s="9"/>
+      <c r="N35" s="9"/>
+    </row>
+    <row r="36" spans="2:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="9"/>
+    </row>
+    <row r="37" spans="2:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="9"/>
+      <c r="M37" s="9"/>
+      <c r="N37" s="9"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>